<commit_message>
UPdated titles and fixed geom_text
</commit_message>
<xml_diff>
--- a/contratoguia - worksheets.xlsx
+++ b/contratoguia - worksheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b353020857715e37/Desktop/R_Projects/central_am_migration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenis\OneDrive\Desktop\R_Projects\central_am_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{94433239-7C18-7E43-B703-07CD705EFBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3884BFD-578F-4B5F-997D-60BEB6280FB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237950C-5911-44B2-B821-FAAA82C3AAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moneda conversion table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="101">
   <si>
     <t>Ano</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>adj_perc</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -381,6 +384,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -590,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -739,6 +748,7 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3203,9 +3213,9 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3273,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="1"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2019</v>
       </c>
@@ -3317,7 +3327,7 @@
       <c r="V2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -3371,7 +3381,7 @@
       <c r="V3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2017</v>
       </c>
@@ -3421,7 +3431,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2016</v>
       </c>
@@ -3471,7 +3481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
@@ -3521,7 +3531,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2014</v>
       </c>
@@ -3571,7 +3581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -3621,7 +3631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2012</v>
       </c>
@@ -3671,7 +3681,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2011</v>
       </c>
@@ -3721,7 +3731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -3731,7 +3741,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -3741,57 +3751,57 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="26"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="26"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="26"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="26"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="26"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="26"/>
@@ -3806,230 +3816,261 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
-      <c r="B2" s="101">
+      <c r="B2" s="102">
+        <v>49</v>
+      </c>
+      <c r="C2" s="101">
         <v>47.39</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>21.3</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>2470</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>1110</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>5212</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
-      <c r="B3" s="101">
+      <c r="B3" s="102">
+        <v>47</v>
+      </c>
+      <c r="C3" s="101">
         <v>45.15</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>54.71</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>2608</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>3160</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>5776</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2013</v>
       </c>
-      <c r="B4" s="101">
+      <c r="B4" s="102">
+        <v>56</v>
+      </c>
+      <c r="C4" s="101">
         <v>53.72</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>45.7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>3751</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>3191</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>6982</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2014</v>
       </c>
-      <c r="B5" s="101">
+      <c r="B5" s="102">
+        <v>58</v>
+      </c>
+      <c r="C5" s="101">
         <v>55.57</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>43.49</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>3570</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>2794</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>6424</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
-      <c r="B6" s="101">
+      <c r="B6" s="102">
+        <v>59</v>
+      </c>
+      <c r="C6" s="101">
         <v>56.86</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>42.72</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>2855</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>2145</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>5021</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
-      <c r="B7" s="101">
+      <c r="B7" s="102">
+        <v>63</v>
+      </c>
+      <c r="C7" s="101">
         <v>60.94</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>37.97</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>2735</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>1704</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>4488</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
-      <c r="B8" s="101">
+      <c r="B8" s="102">
+        <v>61</v>
+      </c>
+      <c r="C8" s="101">
         <v>59.19</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>39.46</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>2587</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>1725</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>4371</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
-      <c r="B9" s="101">
+      <c r="B9" s="102">
+        <v>60</v>
+      </c>
+      <c r="C9" s="101">
         <v>57.71</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="5">
         <v>40.450000000000003</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <v>2290</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>1605</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>3968</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
-      <c r="B10" s="101">
+      <c r="B10" s="102">
+        <v>52</v>
+      </c>
+      <c r="C10" s="101">
         <v>50.14</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>48.1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>882</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>846</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>1759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="10">
-        <f t="shared" ref="D11:F11" si="0">SUM(D2:D10)</f>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="10">
+        <f t="shared" ref="E11:G11" si="0">SUM(E2:E10)</f>
         <v>23748</v>
       </c>
-      <c r="E11" s="10">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>18280</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>44001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4042,9 +4083,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4054,7 +4095,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -4110,7 +4151,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>2011</v>
       </c>
@@ -4163,7 +4204,7 @@
         <v>57.48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>2011</v>
       </c>
@@ -4222,7 +4263,7 @@
         <v>60.77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>2011</v>
       </c>
@@ -4275,7 +4316,7 @@
         <v>22.25</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33">
         <v>2011</v>
       </c>
@@ -4328,7 +4369,7 @@
         <v>50.14</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>2012</v>
       </c>
@@ -4369,7 +4410,7 @@
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <v>2012</v>
       </c>
@@ -4404,7 +4445,7 @@
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44">
         <v>2012</v>
       </c>
@@ -4439,7 +4480,7 @@
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55">
         <v>2012</v>
       </c>
@@ -4471,7 +4512,7 @@
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>2013</v>
       </c>
@@ -4506,7 +4547,7 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>2013</v>
       </c>
@@ -4538,7 +4579,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28">
         <v>2013</v>
       </c>
@@ -4570,7 +4611,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33">
         <v>2013</v>
       </c>
@@ -4599,7 +4640,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38">
         <v>2014</v>
       </c>
@@ -4631,7 +4672,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="44">
         <v>2014</v>
       </c>
@@ -4663,7 +4704,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44">
         <v>2014</v>
       </c>
@@ -4695,7 +4736,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="55">
         <v>2014</v>
       </c>
@@ -4724,7 +4765,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>2015</v>
       </c>
@@ -4756,7 +4797,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>2015</v>
       </c>
@@ -4788,7 +4829,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28">
         <v>2015</v>
       </c>
@@ -4820,7 +4861,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33">
         <v>2015</v>
       </c>
@@ -4849,7 +4890,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="38">
         <v>2016</v>
       </c>
@@ -4881,7 +4922,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>2016</v>
       </c>
@@ -4913,7 +4954,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44">
         <v>2016</v>
       </c>
@@ -4945,7 +4986,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55">
         <v>2016</v>
       </c>
@@ -4974,7 +5015,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>2017</v>
       </c>
@@ -5006,7 +5047,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>2017</v>
       </c>
@@ -5038,7 +5079,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28">
         <v>2017</v>
       </c>
@@ -5070,7 +5111,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33">
         <v>2017</v>
       </c>
@@ -5099,7 +5140,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38">
         <v>2018</v>
       </c>
@@ -5131,7 +5172,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>2018</v>
       </c>
@@ -5163,7 +5204,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44">
         <v>2018</v>
       </c>
@@ -5195,7 +5236,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="55">
         <v>2018</v>
       </c>
@@ -5224,7 +5265,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28">
         <v>2019</v>
       </c>
@@ -5256,7 +5297,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28">
         <v>2019</v>
       </c>
@@ -5288,7 +5329,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28">
         <v>2019</v>
       </c>
@@ -5320,7 +5361,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33">
         <v>2019</v>
       </c>
@@ -5349,7 +5390,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -5358,7 +5399,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -5367,7 +5408,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -5376,7 +5417,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -5385,7 +5426,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -5394,7 +5435,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -5403,7 +5444,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -5412,7 +5453,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -5421,7 +5462,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -5430,7 +5471,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -5439,7 +5480,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -5448,7 +5489,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -5457,7 +5498,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -5466,7 +5507,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -5475,7 +5516,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -5484,7 +5525,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -5493,7 +5534,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -5502,7 +5543,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -5511,7 +5552,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -5520,7 +5561,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -5529,7 +5570,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -5538,7 +5579,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -5547,7 +5588,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -5556,7 +5597,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -5565,7 +5606,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -5574,7 +5615,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -5583,7 +5624,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -5592,7 +5633,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -5601,7 +5642,7 @@
       <c r="H69" s="80"/>
       <c r="I69" s="80"/>
     </row>
-    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="80"/>
       <c r="D70" s="80"/>
       <c r="E70" s="80"/>
@@ -5610,7 +5651,7 @@
       <c r="H70" s="80"/>
       <c r="I70" s="80"/>
     </row>
-    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="80"/>
       <c r="D71" s="80"/>
       <c r="E71" s="80"/>
@@ -5619,7 +5660,7 @@
       <c r="H71" s="80"/>
       <c r="I71" s="80"/>
     </row>
-    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="80"/>
       <c r="D72" s="80"/>
       <c r="E72" s="80"/>
@@ -5628,7 +5669,7 @@
       <c r="H72" s="80"/>
       <c r="I72" s="80"/>
     </row>
-    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="80"/>
       <c r="D73" s="80"/>
       <c r="E73" s="80"/>
@@ -5652,9 +5693,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5665,7 +5706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -5715,7 +5756,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>2012</v>
       </c>
@@ -5768,7 +5809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>2012</v>
       </c>
@@ -5821,7 +5862,7 @@
         <v>56.65</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -5842,7 +5883,7 @@
       <c r="T8" s="56"/>
       <c r="U8" s="56"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -5863,7 +5904,7 @@
       <c r="T9" s="56"/>
       <c r="U9" s="56"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>2013</v>
       </c>
@@ -5898,7 +5939,7 @@
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <v>2013</v>
       </c>
@@ -5926,7 +5967,7 @@
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="30"/>
       <c r="E12" s="47"/>
@@ -5936,7 +5977,7 @@
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="35"/>
       <c r="C13" s="58"/>
@@ -5951,7 +5992,7 @@
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>2014</v>
       </c>
@@ -5980,7 +6021,7 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>2014</v>
       </c>
@@ -6006,7 +6047,7 @@
       <c r="I15" s="30"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -6018,7 +6059,7 @@
       <c r="I16" s="30"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -6030,7 +6071,7 @@
       <c r="I17" s="62"/>
       <c r="J17" s="63"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38">
         <v>2015</v>
       </c>
@@ -6056,7 +6097,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="44">
         <v>2015</v>
       </c>
@@ -6081,13 +6122,13 @@
       <c r="H19" s="44"/>
       <c r="J19" s="50"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
       <c r="B20" s="30"/>
       <c r="H20" s="44"/>
       <c r="J20" s="50"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="55"/>
       <c r="B21" s="35"/>
       <c r="C21" s="58"/>
@@ -6099,7 +6140,7 @@
       <c r="I21" s="65"/>
       <c r="J21" s="66"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>2016</v>
       </c>
@@ -6125,7 +6166,7 @@
       <c r="I22" s="19"/>
       <c r="J22" s="23"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>2016</v>
       </c>
@@ -6151,7 +6192,7 @@
       <c r="I23" s="30"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28"/>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -6163,7 +6204,7 @@
       <c r="I24" s="30"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
@@ -6175,7 +6216,7 @@
       <c r="I25" s="62"/>
       <c r="J25" s="63"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="38">
         <v>2017</v>
       </c>
@@ -6201,7 +6242,7 @@
       <c r="I26" s="40"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>2017</v>
       </c>
@@ -6226,13 +6267,13 @@
       <c r="H27" s="44"/>
       <c r="J27" s="50"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="30"/>
       <c r="H28" s="44"/>
       <c r="J28" s="50"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
       <c r="B29" s="35"/>
       <c r="C29" s="58"/>
@@ -6244,7 +6285,7 @@
       <c r="I29" s="65"/>
       <c r="J29" s="66"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>2018</v>
       </c>
@@ -6270,7 +6311,7 @@
       <c r="I30" s="19"/>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>2018</v>
       </c>
@@ -6296,7 +6337,7 @@
       <c r="I31" s="30"/>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -6308,7 +6349,7 @@
       <c r="I32" s="30"/>
       <c r="J32" s="32"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
@@ -6320,7 +6361,7 @@
       <c r="I33" s="62"/>
       <c r="J33" s="63"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38">
         <v>2019</v>
       </c>
@@ -6346,7 +6387,7 @@
       <c r="I34" s="40"/>
       <c r="J34" s="43"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>2019</v>
       </c>
@@ -6371,13 +6412,13 @@
       <c r="H35" s="44"/>
       <c r="J35" s="50"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44"/>
       <c r="B36" s="30"/>
       <c r="H36" s="44"/>
       <c r="J36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="55"/>
       <c r="B37" s="58"/>
       <c r="C37" s="58"/>
@@ -6389,7 +6430,7 @@
       <c r="I37" s="65"/>
       <c r="J37" s="66"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -6401,7 +6442,7 @@
       <c r="I38" s="30"/>
       <c r="J38" s="32"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -6413,7 +6454,7 @@
       <c r="I39" s="30"/>
       <c r="J39" s="32"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -6425,7 +6466,7 @@
       <c r="I40" s="30"/>
       <c r="J40" s="32"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35"/>
@@ -6437,7 +6478,7 @@
       <c r="I41" s="62"/>
       <c r="J41" s="63"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -6446,7 +6487,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -6455,7 +6496,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -6464,7 +6505,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -6473,7 +6514,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -6482,7 +6523,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -6491,7 +6532,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -6500,7 +6541,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -6509,7 +6550,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -6518,7 +6559,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -6527,7 +6568,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -6536,7 +6577,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -6545,7 +6586,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -6554,7 +6595,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -6563,7 +6604,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -6572,7 +6613,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -6581,7 +6622,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -6590,7 +6631,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -6599,7 +6640,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -6608,7 +6649,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -6617,7 +6658,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -6626,7 +6667,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -6635,7 +6676,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -6644,7 +6685,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -6653,7 +6694,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -6662,7 +6703,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -6671,7 +6712,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -6680,7 +6721,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -6689,7 +6730,7 @@
       <c r="H69" s="80"/>
       <c r="I69" s="80"/>
     </row>
-    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="80"/>
       <c r="D70" s="80"/>
       <c r="E70" s="80"/>
@@ -6698,7 +6739,7 @@
       <c r="H70" s="80"/>
       <c r="I70" s="80"/>
     </row>
-    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="80"/>
       <c r="D71" s="80"/>
       <c r="E71" s="80"/>
@@ -6707,7 +6748,7 @@
       <c r="H71" s="80"/>
       <c r="I71" s="80"/>
     </row>
-    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="80"/>
       <c r="D72" s="80"/>
       <c r="E72" s="80"/>
@@ -6716,7 +6757,7 @@
       <c r="H72" s="80"/>
       <c r="I72" s="80"/>
     </row>
-    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="80"/>
       <c r="D73" s="80"/>
       <c r="E73" s="80"/>
@@ -6740,9 +6781,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -6780,7 +6821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>2011</v>
       </c>
@@ -6812,7 +6853,7 @@
       <c r="AA2" s="52"/>
       <c r="AB2" s="52"/>
     </row>
-    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>2011</v>
       </c>
@@ -6900,7 +6941,7 @@
       <c r="AL3" s="78"/>
       <c r="AM3" s="78"/>
     </row>
-    <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>2011</v>
       </c>
@@ -6986,7 +7027,7 @@
       <c r="AL4" s="70"/>
       <c r="AM4" s="70"/>
     </row>
-    <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33">
         <v>2011</v>
       </c>
@@ -7074,7 +7115,7 @@
       <c r="AL5" s="70"/>
       <c r="AM5" s="70"/>
     </row>
-    <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="38">
         <v>2012</v>
       </c>
@@ -7166,7 +7207,7 @@
       <c r="AL6" s="70"/>
       <c r="AM6" s="70"/>
     </row>
-    <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44">
         <v>2012</v>
       </c>
@@ -7273,7 +7314,7 @@
       <c r="AL7" s="96"/>
       <c r="AM7" s="96"/>
     </row>
-    <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44">
         <v>2012</v>
       </c>
@@ -7310,7 +7351,7 @@
       <c r="T8" s="97"/>
       <c r="AC8" s="98"/>
     </row>
-    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55">
         <v>2012</v>
       </c>
@@ -7348,7 +7389,7 @@
       <c r="N9" s="52"/>
       <c r="O9" s="52"/>
     </row>
-    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>2013</v>
       </c>
@@ -7383,7 +7424,7 @@
       <c r="N10" s="52"/>
       <c r="O10" s="52"/>
     </row>
-    <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>2013</v>
       </c>
@@ -7415,7 +7456,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>2013</v>
       </c>
@@ -7447,7 +7488,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33">
         <v>2013</v>
       </c>
@@ -7482,7 +7523,7 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>2014</v>
       </c>
@@ -7514,7 +7555,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="44">
         <v>2014</v>
       </c>
@@ -7546,7 +7587,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44">
         <v>2014</v>
       </c>
@@ -7578,7 +7619,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="55">
         <v>2014</v>
       </c>
@@ -7613,7 +7654,7 @@
         <v>3340</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>2015</v>
       </c>
@@ -7645,7 +7686,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <v>2015</v>
       </c>
@@ -7677,7 +7718,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28">
         <v>2015</v>
       </c>
@@ -7709,7 +7750,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33">
         <v>2015</v>
       </c>
@@ -7744,7 +7785,7 @@
         <v>2692</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38">
         <v>2016</v>
       </c>
@@ -7776,7 +7817,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44">
         <v>2016</v>
       </c>
@@ -7808,7 +7849,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44">
         <v>2016</v>
       </c>
@@ -7840,7 +7881,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="55">
         <v>2016</v>
       </c>
@@ -7875,7 +7916,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17">
         <v>2017</v>
       </c>
@@ -7907,7 +7948,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28">
         <v>2017</v>
       </c>
@@ -7939,7 +7980,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28">
         <v>2017</v>
       </c>
@@ -7971,7 +8012,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="33">
         <v>2017</v>
       </c>
@@ -8006,7 +8047,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38">
         <v>2018</v>
       </c>
@@ -8038,7 +8079,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="44">
         <v>2018</v>
       </c>
@@ -8070,7 +8111,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <v>2018</v>
       </c>
@@ -8102,7 +8143,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="55">
         <v>2018</v>
       </c>
@@ -8137,7 +8178,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28">
         <v>2019</v>
       </c>
@@ -8169,7 +8210,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28">
         <v>2019</v>
       </c>
@@ -8201,7 +8242,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28">
         <v>2019</v>
       </c>
@@ -8233,7 +8274,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="33">
         <v>2019</v>
       </c>
@@ -8268,7 +8309,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="80"/>
       <c r="D38" s="80"/>
       <c r="E38" s="80"/>
@@ -8277,7 +8318,7 @@
       <c r="H38" s="80"/>
       <c r="I38" s="80"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="80"/>
       <c r="D39" s="80"/>
       <c r="E39" s="80"/>
@@ -8286,7 +8327,7 @@
       <c r="H39" s="80"/>
       <c r="I39" s="80"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="80"/>
       <c r="D40" s="80"/>
       <c r="E40" s="80"/>
@@ -8295,7 +8336,7 @@
       <c r="H40" s="80"/>
       <c r="I40" s="80"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="80"/>
       <c r="D41" s="80"/>
       <c r="E41" s="80"/>
@@ -8304,7 +8345,7 @@
       <c r="H41" s="80"/>
       <c r="I41" s="80"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -8313,7 +8354,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -8322,7 +8363,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -8331,7 +8372,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -8340,7 +8381,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -8349,7 +8390,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -8358,7 +8399,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -8367,7 +8408,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -8376,7 +8417,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -8385,7 +8426,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -8394,7 +8435,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -8403,7 +8444,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -8412,7 +8453,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -8421,7 +8462,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -8430,7 +8471,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -8439,7 +8480,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -8448,7 +8489,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -8457,7 +8498,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -8466,7 +8507,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -8475,7 +8516,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -8484,7 +8525,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -8493,7 +8534,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -8502,7 +8543,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -8511,7 +8552,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -8520,7 +8561,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -8529,7 +8570,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -8538,7 +8579,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -8547,7 +8588,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -8571,759 +8612,759 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
not sure why everythin is uncommited o_O
</commit_message>
<xml_diff>
--- a/contratoguia - worksheets.xlsx
+++ b/contratoguia - worksheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b353020857715e37/Desktop/R_Projects/central_am_migration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tenis\OneDrive\Desktop\R_Projects\central_am_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{94433239-7C18-7E43-B703-07CD705EFBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3884BFD-578F-4B5F-997D-60BEB6280FB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C237950C-5911-44B2-B821-FAAA82C3AAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moneda conversion table" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="101">
   <si>
     <t>Ano</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>adj_perc</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -381,6 +384,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -590,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -739,6 +748,7 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3203,9 +3213,9 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3273,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="1"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2019</v>
       </c>
@@ -3317,7 +3327,7 @@
       <c r="V2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -3371,7 +3381,7 @@
       <c r="V3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2017</v>
       </c>
@@ -3421,7 +3431,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2016</v>
       </c>
@@ -3471,7 +3481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2015</v>
       </c>
@@ -3521,7 +3531,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2014</v>
       </c>
@@ -3571,7 +3581,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2013</v>
       </c>
@@ -3621,7 +3631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2012</v>
       </c>
@@ -3671,7 +3681,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2011</v>
       </c>
@@ -3721,7 +3731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -3731,7 +3741,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -3741,57 +3751,57 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="26"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="26"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="26"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="26"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="26"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="26"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="26"/>
@@ -3806,230 +3816,261 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
-      <c r="B2" s="101">
+      <c r="B2" s="102">
+        <v>49</v>
+      </c>
+      <c r="C2" s="101">
         <v>47.39</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>21.3</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>2470</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>1110</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>5212</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
-      <c r="B3" s="101">
+      <c r="B3" s="102">
+        <v>47</v>
+      </c>
+      <c r="C3" s="101">
         <v>45.15</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>54.71</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>2608</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>3160</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>5776</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2013</v>
       </c>
-      <c r="B4" s="101">
+      <c r="B4" s="102">
+        <v>56</v>
+      </c>
+      <c r="C4" s="101">
         <v>53.72</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>45.7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>3751</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>3191</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>6982</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2014</v>
       </c>
-      <c r="B5" s="101">
+      <c r="B5" s="102">
+        <v>58</v>
+      </c>
+      <c r="C5" s="101">
         <v>55.57</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>43.49</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>3570</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>2794</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>6424</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
-      <c r="B6" s="101">
+      <c r="B6" s="102">
+        <v>59</v>
+      </c>
+      <c r="C6" s="101">
         <v>56.86</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>42.72</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>2855</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>2145</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>5021</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
-      <c r="B7" s="101">
+      <c r="B7" s="102">
+        <v>63</v>
+      </c>
+      <c r="C7" s="101">
         <v>60.94</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>37.97</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>2735</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>1704</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>4488</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
-      <c r="B8" s="101">
+      <c r="B8" s="102">
+        <v>61</v>
+      </c>
+      <c r="C8" s="101">
         <v>59.19</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>39.46</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>2587</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>1725</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>4371</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
-      <c r="B9" s="101">
+      <c r="B9" s="102">
+        <v>60</v>
+      </c>
+      <c r="C9" s="101">
         <v>57.71</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="5">
         <v>40.450000000000003</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <v>2290</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>1605</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>3968</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
-      <c r="B10" s="101">
+      <c r="B10" s="102">
+        <v>52</v>
+      </c>
+      <c r="C10" s="101">
         <v>50.14</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>48.1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>882</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>846</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>1759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="10">
-        <f t="shared" ref="D11:F11" si="0">SUM(D2:D10)</f>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="10">
+        <f t="shared" ref="E11:G11" si="0">SUM(E2:E10)</f>
         <v>23748</v>
       </c>
-      <c r="E11" s="10">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>18280</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="12">
         <f t="shared" si="0"/>
         <v>44001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4042,9 +4083,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4054,7 +4095,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -4110,7 +4151,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>2011</v>
       </c>
@@ -4163,7 +4204,7 @@
         <v>57.48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>2011</v>
       </c>
@@ -4222,7 +4263,7 @@
         <v>60.77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>2011</v>
       </c>
@@ -4275,7 +4316,7 @@
         <v>22.25</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33">
         <v>2011</v>
       </c>
@@ -4328,7 +4369,7 @@
         <v>50.14</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>2012</v>
       </c>
@@ -4369,7 +4410,7 @@
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <v>2012</v>
       </c>
@@ -4404,7 +4445,7 @@
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44">
         <v>2012</v>
       </c>
@@ -4439,7 +4480,7 @@
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55">
         <v>2012</v>
       </c>
@@ -4471,7 +4512,7 @@
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>2013</v>
       </c>
@@ -4506,7 +4547,7 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>2013</v>
       </c>
@@ -4538,7 +4579,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28">
         <v>2013</v>
       </c>
@@ -4570,7 +4611,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33">
         <v>2013</v>
       </c>
@@ -4599,7 +4640,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38">
         <v>2014</v>
       </c>
@@ -4631,7 +4672,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="44">
         <v>2014</v>
       </c>
@@ -4663,7 +4704,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44">
         <v>2014</v>
       </c>
@@ -4695,7 +4736,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="55">
         <v>2014</v>
       </c>
@@ -4724,7 +4765,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>2015</v>
       </c>
@@ -4756,7 +4797,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>2015</v>
       </c>
@@ -4788,7 +4829,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28">
         <v>2015</v>
       </c>
@@ -4820,7 +4861,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33">
         <v>2015</v>
       </c>
@@ -4849,7 +4890,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="38">
         <v>2016</v>
       </c>
@@ -4881,7 +4922,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>2016</v>
       </c>
@@ -4913,7 +4954,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44">
         <v>2016</v>
       </c>
@@ -4945,7 +4986,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55">
         <v>2016</v>
       </c>
@@ -4974,7 +5015,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>2017</v>
       </c>
@@ -5006,7 +5047,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>2017</v>
       </c>
@@ -5038,7 +5079,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28">
         <v>2017</v>
       </c>
@@ -5070,7 +5111,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33">
         <v>2017</v>
       </c>
@@ -5099,7 +5140,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38">
         <v>2018</v>
       </c>
@@ -5131,7 +5172,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>2018</v>
       </c>
@@ -5163,7 +5204,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44">
         <v>2018</v>
       </c>
@@ -5195,7 +5236,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="55">
         <v>2018</v>
       </c>
@@ -5224,7 +5265,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28">
         <v>2019</v>
       </c>
@@ -5256,7 +5297,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28">
         <v>2019</v>
       </c>
@@ -5288,7 +5329,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28">
         <v>2019</v>
       </c>
@@ -5320,7 +5361,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33">
         <v>2019</v>
       </c>
@@ -5349,7 +5390,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -5358,7 +5399,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -5367,7 +5408,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -5376,7 +5417,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -5385,7 +5426,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -5394,7 +5435,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -5403,7 +5444,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -5412,7 +5453,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -5421,7 +5462,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -5430,7 +5471,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -5439,7 +5480,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -5448,7 +5489,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -5457,7 +5498,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -5466,7 +5507,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -5475,7 +5516,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -5484,7 +5525,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -5493,7 +5534,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -5502,7 +5543,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -5511,7 +5552,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -5520,7 +5561,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -5529,7 +5570,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -5538,7 +5579,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -5547,7 +5588,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -5556,7 +5597,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -5565,7 +5606,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -5574,7 +5615,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -5583,7 +5624,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -5592,7 +5633,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -5601,7 +5642,7 @@
       <c r="H69" s="80"/>
       <c r="I69" s="80"/>
     </row>
-    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="80"/>
       <c r="D70" s="80"/>
       <c r="E70" s="80"/>
@@ -5610,7 +5651,7 @@
       <c r="H70" s="80"/>
       <c r="I70" s="80"/>
     </row>
-    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="80"/>
       <c r="D71" s="80"/>
       <c r="E71" s="80"/>
@@ -5619,7 +5660,7 @@
       <c r="H71" s="80"/>
       <c r="I71" s="80"/>
     </row>
-    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="80"/>
       <c r="D72" s="80"/>
       <c r="E72" s="80"/>
@@ -5628,7 +5669,7 @@
       <c r="H72" s="80"/>
       <c r="I72" s="80"/>
     </row>
-    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="80"/>
       <c r="D73" s="80"/>
       <c r="E73" s="80"/>
@@ -5652,9 +5693,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5665,7 +5706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -5715,7 +5756,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>2012</v>
       </c>
@@ -5768,7 +5809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>2012</v>
       </c>
@@ -5821,7 +5862,7 @@
         <v>56.65</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -5842,7 +5883,7 @@
       <c r="T8" s="56"/>
       <c r="U8" s="56"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -5863,7 +5904,7 @@
       <c r="T9" s="56"/>
       <c r="U9" s="56"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38">
         <v>2013</v>
       </c>
@@ -5898,7 +5939,7 @@
       <c r="T10" s="27"/>
       <c r="U10" s="27"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <v>2013</v>
       </c>
@@ -5926,7 +5967,7 @@
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
       <c r="B12" s="30"/>
       <c r="E12" s="47"/>
@@ -5936,7 +5977,7 @@
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="35"/>
       <c r="C13" s="58"/>
@@ -5951,7 +5992,7 @@
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>2014</v>
       </c>
@@ -5980,7 +6021,7 @@
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>2014</v>
       </c>
@@ -6006,7 +6047,7 @@
       <c r="I15" s="30"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -6018,7 +6059,7 @@
       <c r="I16" s="30"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -6030,7 +6071,7 @@
       <c r="I17" s="62"/>
       <c r="J17" s="63"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38">
         <v>2015</v>
       </c>
@@ -6056,7 +6097,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="44">
         <v>2015</v>
       </c>
@@ -6081,13 +6122,13 @@
       <c r="H19" s="44"/>
       <c r="J19" s="50"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
       <c r="B20" s="30"/>
       <c r="H20" s="44"/>
       <c r="J20" s="50"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="55"/>
       <c r="B21" s="35"/>
       <c r="C21" s="58"/>
@@ -6099,7 +6140,7 @@
       <c r="I21" s="65"/>
       <c r="J21" s="66"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>2016</v>
       </c>
@@ -6125,7 +6166,7 @@
       <c r="I22" s="19"/>
       <c r="J22" s="23"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>2016</v>
       </c>
@@ -6151,7 +6192,7 @@
       <c r="I23" s="30"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28"/>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -6163,7 +6204,7 @@
       <c r="I24" s="30"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
@@ -6175,7 +6216,7 @@
       <c r="I25" s="62"/>
       <c r="J25" s="63"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="38">
         <v>2017</v>
       </c>
@@ -6201,7 +6242,7 @@
       <c r="I26" s="40"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>2017</v>
       </c>
@@ -6226,13 +6267,13 @@
       <c r="H27" s="44"/>
       <c r="J27" s="50"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="30"/>
       <c r="H28" s="44"/>
       <c r="J28" s="50"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="55"/>
       <c r="B29" s="35"/>
       <c r="C29" s="58"/>
@@ -6244,7 +6285,7 @@
       <c r="I29" s="65"/>
       <c r="J29" s="66"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>2018</v>
       </c>
@@ -6270,7 +6311,7 @@
       <c r="I30" s="19"/>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>2018</v>
       </c>
@@ -6296,7 +6337,7 @@
       <c r="I31" s="30"/>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -6308,7 +6349,7 @@
       <c r="I32" s="30"/>
       <c r="J32" s="32"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
@@ -6320,7 +6361,7 @@
       <c r="I33" s="62"/>
       <c r="J33" s="63"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38">
         <v>2019</v>
       </c>
@@ -6346,7 +6387,7 @@
       <c r="I34" s="40"/>
       <c r="J34" s="43"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>2019</v>
       </c>
@@ -6371,13 +6412,13 @@
       <c r="H35" s="44"/>
       <c r="J35" s="50"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44"/>
       <c r="B36" s="30"/>
       <c r="H36" s="44"/>
       <c r="J36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="55"/>
       <c r="B37" s="58"/>
       <c r="C37" s="58"/>
@@ -6389,7 +6430,7 @@
       <c r="I37" s="65"/>
       <c r="J37" s="66"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -6401,7 +6442,7 @@
       <c r="I38" s="30"/>
       <c r="J38" s="32"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="28"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -6413,7 +6454,7 @@
       <c r="I39" s="30"/>
       <c r="J39" s="32"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="28"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -6425,7 +6466,7 @@
       <c r="I40" s="30"/>
       <c r="J40" s="32"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35"/>
@@ -6437,7 +6478,7 @@
       <c r="I41" s="62"/>
       <c r="J41" s="63"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -6446,7 +6487,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -6455,7 +6496,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -6464,7 +6505,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -6473,7 +6514,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -6482,7 +6523,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -6491,7 +6532,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -6500,7 +6541,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -6509,7 +6550,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -6518,7 +6559,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -6527,7 +6568,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -6536,7 +6577,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -6545,7 +6586,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -6554,7 +6595,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -6563,7 +6604,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -6572,7 +6613,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -6581,7 +6622,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -6590,7 +6631,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -6599,7 +6640,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -6608,7 +6649,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -6617,7 +6658,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -6626,7 +6667,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -6635,7 +6676,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -6644,7 +6685,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -6653,7 +6694,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -6662,7 +6703,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -6671,7 +6712,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -6680,7 +6721,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -6689,7 +6730,7 @@
       <c r="H69" s="80"/>
       <c r="I69" s="80"/>
     </row>
-    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C70" s="80"/>
       <c r="D70" s="80"/>
       <c r="E70" s="80"/>
@@ -6698,7 +6739,7 @@
       <c r="H70" s="80"/>
       <c r="I70" s="80"/>
     </row>
-    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C71" s="80"/>
       <c r="D71" s="80"/>
       <c r="E71" s="80"/>
@@ -6707,7 +6748,7 @@
       <c r="H71" s="80"/>
       <c r="I71" s="80"/>
     </row>
-    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C72" s="80"/>
       <c r="D72" s="80"/>
       <c r="E72" s="80"/>
@@ -6716,7 +6757,7 @@
       <c r="H72" s="80"/>
       <c r="I72" s="80"/>
     </row>
-    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C73" s="80"/>
       <c r="D73" s="80"/>
       <c r="E73" s="80"/>
@@ -6740,9 +6781,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -6780,7 +6821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>2011</v>
       </c>
@@ -6812,7 +6853,7 @@
       <c r="AA2" s="52"/>
       <c r="AB2" s="52"/>
     </row>
-    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>2011</v>
       </c>
@@ -6900,7 +6941,7 @@
       <c r="AL3" s="78"/>
       <c r="AM3" s="78"/>
     </row>
-    <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28">
         <v>2011</v>
       </c>
@@ -6986,7 +7027,7 @@
       <c r="AL4" s="70"/>
       <c r="AM4" s="70"/>
     </row>
-    <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33">
         <v>2011</v>
       </c>
@@ -7074,7 +7115,7 @@
       <c r="AL5" s="70"/>
       <c r="AM5" s="70"/>
     </row>
-    <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="38">
         <v>2012</v>
       </c>
@@ -7166,7 +7207,7 @@
       <c r="AL6" s="70"/>
       <c r="AM6" s="70"/>
     </row>
-    <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44">
         <v>2012</v>
       </c>
@@ -7273,7 +7314,7 @@
       <c r="AL7" s="96"/>
       <c r="AM7" s="96"/>
     </row>
-    <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44">
         <v>2012</v>
       </c>
@@ -7310,7 +7351,7 @@
       <c r="T8" s="97"/>
       <c r="AC8" s="98"/>
     </row>
-    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55">
         <v>2012</v>
       </c>
@@ -7348,7 +7389,7 @@
       <c r="N9" s="52"/>
       <c r="O9" s="52"/>
     </row>
-    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>2013</v>
       </c>
@@ -7383,7 +7424,7 @@
       <c r="N10" s="52"/>
       <c r="O10" s="52"/>
     </row>
-    <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>2013</v>
       </c>
@@ -7415,7 +7456,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>2013</v>
       </c>
@@ -7447,7 +7488,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33">
         <v>2013</v>
       </c>
@@ -7482,7 +7523,7 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>2014</v>
       </c>
@@ -7514,7 +7555,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="44">
         <v>2014</v>
       </c>
@@ -7546,7 +7587,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44">
         <v>2014</v>
       </c>
@@ -7578,7 +7619,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="55">
         <v>2014</v>
       </c>
@@ -7613,7 +7654,7 @@
         <v>3340</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>2015</v>
       </c>
@@ -7645,7 +7686,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <v>2015</v>
       </c>
@@ -7677,7 +7718,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28">
         <v>2015</v>
       </c>
@@ -7709,7 +7750,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33">
         <v>2015</v>
       </c>
@@ -7744,7 +7785,7 @@
         <v>2692</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38">
         <v>2016</v>
       </c>
@@ -7776,7 +7817,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="44">
         <v>2016</v>
       </c>
@@ -7808,7 +7849,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44">
         <v>2016</v>
       </c>
@@ -7840,7 +7881,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="55">
         <v>2016</v>
       </c>
@@ -7875,7 +7916,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17">
         <v>2017</v>
       </c>
@@ -7907,7 +7948,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="28">
         <v>2017</v>
       </c>
@@ -7939,7 +7980,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="28">
         <v>2017</v>
       </c>
@@ -7971,7 +8012,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="33">
         <v>2017</v>
       </c>
@@ -8006,7 +8047,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38">
         <v>2018</v>
       </c>
@@ -8038,7 +8079,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="44">
         <v>2018</v>
       </c>
@@ -8070,7 +8111,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <v>2018</v>
       </c>
@@ -8102,7 +8143,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="55">
         <v>2018</v>
       </c>
@@ -8137,7 +8178,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28">
         <v>2019</v>
       </c>
@@ -8169,7 +8210,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28">
         <v>2019</v>
       </c>
@@ -8201,7 +8242,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28">
         <v>2019</v>
       </c>
@@ -8233,7 +8274,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="33">
         <v>2019</v>
       </c>
@@ -8268,7 +8309,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="80"/>
       <c r="D38" s="80"/>
       <c r="E38" s="80"/>
@@ -8277,7 +8318,7 @@
       <c r="H38" s="80"/>
       <c r="I38" s="80"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="80"/>
       <c r="D39" s="80"/>
       <c r="E39" s="80"/>
@@ -8286,7 +8327,7 @@
       <c r="H39" s="80"/>
       <c r="I39" s="80"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="80"/>
       <c r="D40" s="80"/>
       <c r="E40" s="80"/>
@@ -8295,7 +8336,7 @@
       <c r="H40" s="80"/>
       <c r="I40" s="80"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="80"/>
       <c r="D41" s="80"/>
       <c r="E41" s="80"/>
@@ -8304,7 +8345,7 @@
       <c r="H41" s="80"/>
       <c r="I41" s="80"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
       <c r="E42" s="80"/>
@@ -8313,7 +8354,7 @@
       <c r="H42" s="80"/>
       <c r="I42" s="80"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="80"/>
       <c r="D43" s="80"/>
       <c r="E43" s="80"/>
@@ -8322,7 +8363,7 @@
       <c r="H43" s="80"/>
       <c r="I43" s="80"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
       <c r="E44" s="80"/>
@@ -8331,7 +8372,7 @@
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C45" s="80"/>
       <c r="D45" s="80"/>
       <c r="E45" s="80"/>
@@ -8340,7 +8381,7 @@
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="80"/>
       <c r="D46" s="80"/>
       <c r="E46" s="80"/>
@@ -8349,7 +8390,7 @@
       <c r="H46" s="80"/>
       <c r="I46" s="80"/>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
       <c r="E47" s="80"/>
@@ -8358,7 +8399,7 @@
       <c r="H47" s="80"/>
       <c r="I47" s="80"/>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
       <c r="E48" s="80"/>
@@ -8367,7 +8408,7 @@
       <c r="H48" s="80"/>
       <c r="I48" s="80"/>
     </row>
-    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="80"/>
       <c r="D49" s="80"/>
       <c r="E49" s="80"/>
@@ -8376,7 +8417,7 @@
       <c r="H49" s="80"/>
       <c r="I49" s="80"/>
     </row>
-    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="80"/>
@@ -8385,7 +8426,7 @@
       <c r="H50" s="80"/>
       <c r="I50" s="80"/>
     </row>
-    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
       <c r="E51" s="80"/>
@@ -8394,7 +8435,7 @@
       <c r="H51" s="80"/>
       <c r="I51" s="80"/>
     </row>
-    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="80"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -8403,7 +8444,7 @@
       <c r="H52" s="80"/>
       <c r="I52" s="80"/>
     </row>
-    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
       <c r="E53" s="80"/>
@@ -8412,7 +8453,7 @@
       <c r="H53" s="80"/>
       <c r="I53" s="80"/>
     </row>
-    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="80"/>
@@ -8421,7 +8462,7 @@
       <c r="H54" s="80"/>
       <c r="I54" s="80"/>
     </row>
-    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="80"/>
@@ -8430,7 +8471,7 @@
       <c r="H55" s="80"/>
       <c r="I55" s="80"/>
     </row>
-    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="80"/>
       <c r="D56" s="80"/>
       <c r="E56" s="80"/>
@@ -8439,7 +8480,7 @@
       <c r="H56" s="80"/>
       <c r="I56" s="80"/>
     </row>
-    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="80"/>
       <c r="D57" s="80"/>
       <c r="E57" s="80"/>
@@ -8448,7 +8489,7 @@
       <c r="H57" s="80"/>
       <c r="I57" s="80"/>
     </row>
-    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
       <c r="E58" s="80"/>
@@ -8457,7 +8498,7 @@
       <c r="H58" s="80"/>
       <c r="I58" s="80"/>
     </row>
-    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="80"/>
@@ -8466,7 +8507,7 @@
       <c r="H59" s="80"/>
       <c r="I59" s="80"/>
     </row>
-    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="80"/>
@@ -8475,7 +8516,7 @@
       <c r="H60" s="80"/>
       <c r="I60" s="80"/>
     </row>
-    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="80"/>
       <c r="D61" s="80"/>
       <c r="E61" s="80"/>
@@ -8484,7 +8525,7 @@
       <c r="H61" s="80"/>
       <c r="I61" s="80"/>
     </row>
-    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="80"/>
       <c r="D62" s="80"/>
       <c r="E62" s="80"/>
@@ -8493,7 +8534,7 @@
       <c r="H62" s="80"/>
       <c r="I62" s="80"/>
     </row>
-    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="80"/>
       <c r="D63" s="80"/>
       <c r="E63" s="80"/>
@@ -8502,7 +8543,7 @@
       <c r="H63" s="80"/>
       <c r="I63" s="80"/>
     </row>
-    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
       <c r="E64" s="80"/>
@@ -8511,7 +8552,7 @@
       <c r="H64" s="80"/>
       <c r="I64" s="80"/>
     </row>
-    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
       <c r="E65" s="80"/>
@@ -8520,7 +8561,7 @@
       <c r="H65" s="80"/>
       <c r="I65" s="80"/>
     </row>
-    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C66" s="80"/>
       <c r="D66" s="80"/>
       <c r="E66" s="80"/>
@@ -8529,7 +8570,7 @@
       <c r="H66" s="80"/>
       <c r="I66" s="80"/>
     </row>
-    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C67" s="80"/>
       <c r="D67" s="80"/>
       <c r="E67" s="80"/>
@@ -8538,7 +8579,7 @@
       <c r="H67" s="80"/>
       <c r="I67" s="80"/>
     </row>
-    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C68" s="80"/>
       <c r="D68" s="80"/>
       <c r="E68" s="80"/>
@@ -8547,7 +8588,7 @@
       <c r="H68" s="80"/>
       <c r="I68" s="80"/>
     </row>
-    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C69" s="80"/>
       <c r="D69" s="80"/>
       <c r="E69" s="80"/>
@@ -8571,759 +8612,759 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
         <v>45</v>
       </c>

</xml_diff>